<commit_message>
decimales y estatico 3 piedras
</commit_message>
<xml_diff>
--- a/back-end/Web Dinamico 2/MRVMinem/Documentos/1.1 Plantilla_Etiquetado_de_eficiencia_ Calentadores_ agua_instantaneo.xlsx
+++ b/back-end/Web Dinamico 2/MRVMinem/Documentos/1.1 Plantilla_Etiquetado_de_eficiencia_ Calentadores_ agua_instantaneo.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE9777FF-B67C-4707-A9DB-0D5C9A108A11}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A8E31AF-E404-41F5-A777-CE7C92C25705}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{0FF7017A-1C1F-4F31-834A-BE5FD5CEB108}"/>
   </bookViews>
   <sheets>
     <sheet name="Calentador de agua electrico" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
+    <sheet name="Hoja2" sheetId="2" state="hidden" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="Lista_Anno">Hoja2!$A$5:$A$25</definedName>
@@ -581,7 +581,7 @@
   <dimension ref="A1:F310"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>